<commit_message>
Importación y exportación Clientes
</commit_message>
<xml_diff>
--- a/Clientes.xlsx
+++ b/Clientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\Nana&amp;Rene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4E15D4-0CA3-41EB-81AD-E918CA7376F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED08429-01E9-4B54-8F36-06BDE5AEDD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4176" yWindow="3252" windowWidth="17280" windowHeight="8964" xr2:uid="{22861B7A-0619-407C-A736-D026C188EAA8}"/>
+    <workbookView xWindow="9060" yWindow="2676" windowWidth="17280" windowHeight="8904" xr2:uid="{22861B7A-0619-407C-A736-D026C188EAA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -63,21 +63,6 @@
     <t>limau@gmail.com</t>
   </si>
   <si>
-    <t>4 pies</t>
-  </si>
-  <si>
-    <t>5 tartaletas</t>
-  </si>
-  <si>
-    <t>3 queques</t>
-  </si>
-  <si>
-    <t>2 tortaas</t>
-  </si>
-  <si>
-    <t>1 torta</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -88,6 +73,21 @@
   </si>
   <si>
     <t>Número telefónico</t>
+  </si>
+  <si>
+    <t>1-torta,</t>
+  </si>
+  <si>
+    <t>2-torta,</t>
+  </si>
+  <si>
+    <t>3-queque,</t>
+  </si>
+  <si>
+    <t>4-pie de limon,</t>
+  </si>
+  <si>
+    <t>5-tartaleta durazno,</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,16 +469,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>948274758</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -520,7 +520,7 @@
         <v>946284475</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -534,7 +534,7 @@
         <v>987393274</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -548,7 +548,7 @@
         <v>987452784</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -560,5 +560,6 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{03D6587D-A756-4488-8686-895B30E71A3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>